<commit_message>
udemy features file practice
</commit_message>
<xml_diff>
--- a/src/SampleData555.xlsx
+++ b/src/SampleData555.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitali\IdeaProjects\chicago10cucumberjunit\src\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>FirstName</t>
   </si>
@@ -94,12 +94,16 @@
   </si>
   <si>
     <t>SDET</t>
+  </si>
+  <si>
+    <t>Madam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,8 +457,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -506,7 +510,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -514,7 +518,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>

</xml_diff>